<commit_message>
Update for Night 2
</commit_message>
<xml_diff>
--- a/DNC_FantasyLeague/DNC_FantasyStandings.xlsx
+++ b/DNC_FantasyLeague/DNC_FantasyStandings.xlsx
@@ -13,8 +13,8 @@
     <sheet name="By Speaker" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'By Night'!$A$1:$B$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'By Speaker'!$A$1:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'By Night'!$A$1:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'By Speaker'!$A$1:$D$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'By Word'!$A$1:$C$62</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Standings!$A$1:$B$9</definedName>
   </definedNames>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="77">
   <si>
     <t>Player</t>
   </si>
@@ -58,43 +58,52 @@
     <t>Word</t>
   </si>
   <si>
+    <t>family</t>
+  </si>
+  <si>
     <t>pandemic</t>
   </si>
   <si>
     <t>families</t>
   </si>
   <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>working</t>
+  </si>
+  <si>
     <t>job</t>
   </si>
   <si>
-    <t>change</t>
-  </si>
-  <si>
     <t>leaders</t>
   </si>
   <si>
-    <t>working</t>
+    <t>leadership</t>
+  </si>
+  <si>
+    <t>economy</t>
+  </si>
+  <si>
+    <t>climate</t>
   </si>
   <si>
     <t>hope</t>
   </si>
   <si>
-    <t>economy</t>
-  </si>
-  <si>
-    <t>climate</t>
+    <t>social security</t>
+  </si>
+  <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>communities</t>
   </si>
   <si>
     <t>economic</t>
   </si>
   <si>
-    <t>family</t>
-  </si>
-  <si>
-    <t>progress</t>
-  </si>
-  <si>
-    <t>social security</t>
+    <t>soul</t>
   </si>
   <si>
     <t>racism</t>
@@ -103,27 +112,24 @@
     <t>jobs</t>
   </si>
   <si>
+    <t>science</t>
+  </si>
+  <si>
     <t>scientists</t>
   </si>
   <si>
-    <t>science</t>
+    <t>barack</t>
+  </si>
+  <si>
+    <t>community</t>
+  </si>
+  <si>
+    <t>lewis</t>
   </si>
   <si>
     <t>police</t>
   </si>
   <si>
-    <t>lewis</t>
-  </si>
-  <si>
-    <t>communities</t>
-  </si>
-  <si>
-    <t>barack</t>
-  </si>
-  <si>
-    <t>leadership</t>
-  </si>
-  <si>
     <t>corporations</t>
   </si>
   <si>
@@ -136,12 +142,12 @@
     <t>billionaires</t>
   </si>
   <si>
-    <t>soul</t>
-  </si>
-  <si>
     <t>mail</t>
   </si>
   <si>
+    <t>first responders</t>
+  </si>
+  <si>
     <t>scientific</t>
   </si>
   <si>
@@ -157,94 +163,94 @@
     <t>essential workers</t>
   </si>
   <si>
-    <t>first responders</t>
-  </si>
-  <si>
     <t>middle class</t>
   </si>
   <si>
     <t>scientist</t>
   </si>
   <si>
+    <t>experts</t>
+  </si>
+  <si>
+    <t>build back</t>
+  </si>
+  <si>
+    <t>covid</t>
+  </si>
+  <si>
+    <t>leader</t>
+  </si>
+  <si>
+    <t>obamacare</t>
+  </si>
+  <si>
+    <t>corporate</t>
+  </si>
+  <si>
+    <t>changed</t>
+  </si>
+  <si>
+    <t>expert</t>
+  </si>
+  <si>
+    <t>changing</t>
+  </si>
+  <si>
+    <t>unity</t>
+  </si>
+  <si>
+    <t>unites</t>
+  </si>
+  <si>
+    <t>unite</t>
+  </si>
+  <si>
+    <t>tough</t>
+  </si>
+  <si>
+    <t>progressive</t>
+  </si>
+  <si>
+    <t>defund</t>
+  </si>
+  <si>
+    <t>healthcare</t>
+  </si>
+  <si>
+    <t>recovery act</t>
+  </si>
+  <si>
+    <t>hopes</t>
+  </si>
+  <si>
+    <t>hoping</t>
+  </si>
+  <si>
+    <t>fighter</t>
+  </si>
+  <si>
+    <t>policing</t>
+  </si>
+  <si>
+    <t>obama</t>
+  </si>
+  <si>
+    <t>malarkey</t>
+  </si>
+  <si>
     <t>changes</t>
   </si>
   <si>
-    <t>build back</t>
-  </si>
-  <si>
-    <t>covid</t>
-  </si>
-  <si>
-    <t>leader</t>
-  </si>
-  <si>
-    <t>obamacare</t>
-  </si>
-  <si>
-    <t>corporate</t>
-  </si>
-  <si>
-    <t>changed</t>
-  </si>
-  <si>
-    <t>malarkey</t>
-  </si>
-  <si>
-    <t>experts</t>
-  </si>
-  <si>
-    <t>hopes</t>
-  </si>
-  <si>
-    <t>expert</t>
-  </si>
-  <si>
-    <t>obama</t>
-  </si>
-  <si>
-    <t>fighter</t>
-  </si>
-  <si>
-    <t>policing</t>
-  </si>
-  <si>
-    <t>recovery act</t>
-  </si>
-  <si>
-    <t>hoping</t>
-  </si>
-  <si>
-    <t>tough</t>
-  </si>
-  <si>
-    <t>unity</t>
-  </si>
-  <si>
-    <t>healthcare</t>
-  </si>
-  <si>
-    <t>defund</t>
-  </si>
-  <si>
-    <t>progressive</t>
-  </si>
-  <si>
-    <t>unite</t>
-  </si>
-  <si>
-    <t>community</t>
-  </si>
-  <si>
-    <t>unites</t>
-  </si>
-  <si>
-    <t>changing</t>
-  </si>
-  <si>
     <t>Night1</t>
   </si>
   <si>
+    <t>Night2</t>
+  </si>
+  <si>
     <t>BernieSanders</t>
+  </si>
+  <si>
+    <t>JillBiden</t>
   </si>
   <si>
     <t>MichelleObama</t>
@@ -631,7 +637,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -639,7 +645,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -647,7 +653,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -655,7 +661,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -663,7 +669,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -687,7 +693,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -734,24 +740,24 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -762,7 +768,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -773,7 +779,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -784,45 +790,45 @@
         <v>15</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
@@ -833,7 +839,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>
@@ -844,7 +850,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>21</v>
@@ -855,7 +861,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>22</v>
@@ -866,7 +872,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>23</v>
@@ -877,29 +883,29 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>26</v>
@@ -910,7 +916,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>27</v>
@@ -921,35 +927,35 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -965,7 +971,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>32</v>
@@ -976,7 +982,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>33</v>
@@ -998,7 +1004,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>35</v>
@@ -1009,7 +1015,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>36</v>
@@ -1020,7 +1026,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>37</v>
@@ -1031,7 +1037,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>38</v>
@@ -1042,13 +1048,13 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1059,12 +1065,12 @@
         <v>40</v>
       </c>
       <c r="C31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>41</v>
@@ -1075,7 +1081,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>42</v>
@@ -1086,7 +1092,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>43</v>
@@ -1097,7 +1103,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>44</v>
@@ -1130,7 +1136,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>47</v>
@@ -1141,7 +1147,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>48</v>
@@ -1163,7 +1169,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>50</v>
@@ -1174,7 +1180,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>51</v>
@@ -1185,7 +1191,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>52</v>
@@ -1196,7 +1202,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>53</v>
@@ -1207,7 +1213,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>54</v>
@@ -1229,7 +1235,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>56</v>
@@ -1240,7 +1246,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>57</v>
@@ -1251,7 +1257,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>58</v>
@@ -1273,7 +1279,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>60</v>
@@ -1284,7 +1290,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>61</v>
@@ -1306,7 +1312,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>63</v>
@@ -1350,7 +1356,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>67</v>
@@ -1361,7 +1367,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>68</v>
@@ -1372,7 +1378,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>69</v>
@@ -1383,7 +1389,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>70</v>
@@ -1423,7 +1429,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1431,89 +1437,117 @@
   <cols>
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
       </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B9"/>
+  <autoFilter ref="A1:C9"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1521,21 +1555,25 @@
   <cols>
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>75</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1543,10 +1581,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1554,10 +1595,13 @@
         <v>9</v>
       </c>
       <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1565,10 +1609,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1576,10 +1623,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1589,8 +1639,11 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1600,8 +1653,11 @@
       <c r="C7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1609,10 +1665,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1620,11 +1679,14 @@
         <v>5</v>
       </c>
       <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C9"/>
+  <autoFilter ref="A1:D9"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Night 4 DNC Update
</commit_message>
<xml_diff>
--- a/DNC_FantasyLeague/DNC_FantasyStandings.xlsx
+++ b/DNC_FantasyLeague/DNC_FantasyStandings.xlsx
@@ -13,8 +13,8 @@
     <sheet name="By Speaker" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'By Night'!$A$1:$D$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'By Speaker'!$A$1:$F$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'By Night'!$A$1:$E$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'By Speaker'!$A$1:$G$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'By Word'!$A$1:$C$66</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Standings!$A$1:$B$9</definedName>
   </definedNames>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="86">
   <si>
     <t>Player</t>
   </si>
@@ -34,27 +34,27 @@
     <t>Ashley</t>
   </si>
   <si>
+    <t>Jake</t>
+  </si>
+  <si>
+    <t>Joel</t>
+  </si>
+  <si>
     <t>Angela</t>
   </si>
   <si>
-    <t>Jake</t>
+    <t>Priya</t>
   </si>
   <si>
     <t>Shannon</t>
   </si>
   <si>
-    <t>Priya</t>
-  </si>
-  <si>
-    <t>Joel</t>
+    <t>Mike Kim</t>
   </si>
   <si>
     <t>Naoko</t>
   </si>
   <si>
-    <t>Mike Kim</t>
-  </si>
-  <si>
     <t>Word</t>
   </si>
   <si>
@@ -64,195 +64,195 @@
     <t>job</t>
   </si>
   <si>
+    <t>hope</t>
+  </si>
+  <si>
     <t>pandemic</t>
   </si>
   <si>
+    <t>families</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
     <t>working</t>
   </si>
   <si>
-    <t>families</t>
-  </si>
-  <si>
-    <t>change</t>
-  </si>
-  <si>
     <t>economy</t>
   </si>
   <si>
+    <t>jobs</t>
+  </si>
+  <si>
+    <t>climate</t>
+  </si>
+  <si>
+    <t>economic</t>
+  </si>
+  <si>
+    <t>racism</t>
+  </si>
+  <si>
     <t>leadership</t>
   </si>
   <si>
-    <t>racism</t>
+    <t>community</t>
+  </si>
+  <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>social security</t>
+  </si>
+  <si>
+    <t>communities</t>
   </si>
   <si>
     <t>leaders</t>
   </si>
   <si>
-    <t>hope</t>
-  </si>
-  <si>
-    <t>jobs</t>
-  </si>
-  <si>
-    <t>climate</t>
-  </si>
-  <si>
-    <t>progress</t>
-  </si>
-  <si>
-    <t>economic</t>
+    <t>soul</t>
+  </si>
+  <si>
+    <t>lewis</t>
   </si>
   <si>
     <t>science</t>
   </si>
   <si>
-    <t>community</t>
-  </si>
-  <si>
-    <t>communities</t>
-  </si>
-  <si>
-    <t>lewis</t>
-  </si>
-  <si>
-    <t>social security</t>
-  </si>
-  <si>
-    <t>soul</t>
+    <t>affordable care</t>
+  </si>
+  <si>
+    <t>racial</t>
+  </si>
+  <si>
+    <t>corporations</t>
+  </si>
+  <si>
+    <t>obama</t>
+  </si>
+  <si>
+    <t>barack</t>
   </si>
   <si>
     <t>police</t>
   </si>
   <si>
-    <t>barack</t>
-  </si>
-  <si>
     <t>postal</t>
   </si>
   <si>
-    <t>affordable care</t>
+    <t>recovery act</t>
+  </si>
+  <si>
+    <t>back better</t>
   </si>
   <si>
     <t>scientists</t>
   </si>
   <si>
-    <t>recovery act</t>
+    <t>experts</t>
+  </si>
+  <si>
+    <t>essential workers</t>
+  </si>
+  <si>
+    <t>leader</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>covid</t>
+  </si>
+  <si>
+    <t>good trouble</t>
+  </si>
+  <si>
+    <t>middle class</t>
   </si>
   <si>
     <t>first responders</t>
   </si>
   <si>
+    <t>changed</t>
+  </si>
+  <si>
+    <t>changes</t>
+  </si>
+  <si>
+    <t>changing</t>
+  </si>
+  <si>
+    <t>billionaires</t>
+  </si>
+  <si>
+    <t>racist</t>
+  </si>
+  <si>
+    <t>unite</t>
+  </si>
+  <si>
     <t>hoping</t>
   </si>
   <si>
-    <t>corporations</t>
-  </si>
-  <si>
-    <t>leader</t>
-  </si>
-  <si>
-    <t>mail</t>
-  </si>
-  <si>
-    <t>back better</t>
-  </si>
-  <si>
-    <t>good trouble</t>
-  </si>
-  <si>
-    <t>changes</t>
-  </si>
-  <si>
-    <t>billionaires</t>
-  </si>
-  <si>
-    <t>obama</t>
-  </si>
-  <si>
-    <t>racist</t>
-  </si>
-  <si>
-    <t>racial</t>
+    <t>scientist</t>
+  </si>
+  <si>
+    <t>corporate</t>
+  </si>
+  <si>
+    <t>obamacare</t>
+  </si>
+  <si>
+    <t>malarkey</t>
+  </si>
+  <si>
+    <t>fighter</t>
+  </si>
+  <si>
+    <t>policing</t>
+  </si>
+  <si>
+    <t>aca</t>
+  </si>
+  <si>
+    <t>tough</t>
   </si>
   <si>
     <t>unites</t>
   </si>
   <si>
+    <t>unity</t>
+  </si>
+  <si>
+    <t>hopes</t>
+  </si>
+  <si>
     <t>tweet</t>
   </si>
   <si>
-    <t>corporate</t>
-  </si>
-  <si>
-    <t>malarkey</t>
-  </si>
-  <si>
-    <t>obamacare</t>
-  </si>
-  <si>
-    <t>experts</t>
-  </si>
-  <si>
-    <t>covid</t>
+    <t>twitter</t>
+  </si>
+  <si>
+    <t>healthcare</t>
+  </si>
+  <si>
+    <t>defund</t>
   </si>
   <si>
     <t>expert</t>
   </si>
   <si>
-    <t>tough</t>
-  </si>
-  <si>
-    <t>aca</t>
-  </si>
-  <si>
-    <t>unite</t>
-  </si>
-  <si>
-    <t>scientist</t>
-  </si>
-  <si>
-    <t>twitter</t>
-  </si>
-  <si>
-    <t>hopes</t>
+    <t>progressive</t>
+  </si>
+  <si>
+    <t>economies</t>
   </si>
   <si>
     <t>scientific</t>
   </si>
   <si>
-    <t>changed</t>
-  </si>
-  <si>
-    <t>changing</t>
-  </si>
-  <si>
-    <t>middle class</t>
-  </si>
-  <si>
-    <t>policing</t>
-  </si>
-  <si>
-    <t>essential workers</t>
-  </si>
-  <si>
-    <t>economies</t>
-  </si>
-  <si>
-    <t>progressive</t>
-  </si>
-  <si>
-    <t>defund</t>
-  </si>
-  <si>
-    <t>healthcare</t>
-  </si>
-  <si>
-    <t>unity</t>
-  </si>
-  <si>
-    <t>fighter</t>
-  </si>
-  <si>
     <t>Night1</t>
   </si>
   <si>
@@ -262,6 +262,9 @@
     <t>Night3</t>
   </si>
   <si>
+    <t>Night4</t>
+  </si>
+  <si>
     <t>BarackObama</t>
   </si>
   <si>
@@ -269,6 +272,9 @@
   </si>
   <si>
     <t>JillBiden</t>
+  </si>
+  <si>
+    <t>JoeBiden</t>
   </si>
   <si>
     <t>KamalaHarris</t>
@@ -658,7 +664,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -666,7 +672,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -674,7 +680,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -682,7 +688,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -690,7 +696,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -698,7 +704,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -706,7 +712,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -714,7 +720,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -767,7 +773,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="1">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -778,29 +784,29 @@
         <v>12</v>
       </c>
       <c r="C3" s="1">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -811,51 +817,51 @@
         <v>15</v>
       </c>
       <c r="C6" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="1">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -866,128 +872,128 @@
         <v>20</v>
       </c>
       <c r="C11" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -998,18 +1004,18 @@
         <v>32</v>
       </c>
       <c r="C23" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1020,23 +1026,23 @@
         <v>34</v>
       </c>
       <c r="C25" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>36</v>
@@ -1047,7 +1053,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>37</v>
@@ -1058,51 +1064,51 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C30" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>42</v>
@@ -1113,7 +1119,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>43</v>
@@ -1124,7 +1130,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>44</v>
@@ -1135,7 +1141,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>45</v>
@@ -1146,7 +1152,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>46</v>
@@ -1157,7 +1163,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>47</v>
@@ -1168,7 +1174,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>48</v>
@@ -1179,7 +1185,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>49</v>
@@ -1190,24 +1196,24 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C41" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C42" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1218,29 +1224,29 @@
         <v>52</v>
       </c>
       <c r="C43" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C44" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C45" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1251,23 +1257,23 @@
         <v>55</v>
       </c>
       <c r="C46" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>57</v>
@@ -1278,7 +1284,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>58</v>
@@ -1289,7 +1295,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>59</v>
@@ -1311,7 +1317,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>61</v>
@@ -1322,7 +1328,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>62</v>
@@ -1344,7 +1350,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>64</v>
@@ -1355,7 +1361,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>65</v>
@@ -1366,7 +1372,7 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>66</v>
@@ -1377,7 +1383,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>67</v>
@@ -1388,7 +1394,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>68</v>
@@ -1399,7 +1405,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>69</v>
@@ -1410,7 +1416,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>70</v>
@@ -1432,7 +1438,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>72</v>
@@ -1443,7 +1449,7 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>73</v>
@@ -1454,7 +1460,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>74</v>
@@ -1465,7 +1471,7 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>75</v>
@@ -1494,7 +1500,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1504,9 +1510,10 @@
     <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1519,10 +1526,13 @@
       <c r="D1" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>11</v>
@@ -1533,8 +1543,11 @@
       <c r="D2" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1547,10 +1560,13 @@
       <c r="D3" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -1561,10 +1577,13 @@
       <c r="D4" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>7</v>
@@ -1575,25 +1594,31 @@
       <c r="D5" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1603,8 +1628,11 @@
       <c r="D7" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1617,10 +1645,13 @@
       <c r="D8" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -1631,16 +1662,19 @@
       <c r="D9" s="1">
         <v>9</v>
       </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D9"/>
+  <autoFilter ref="A1:E9"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1650,33 +1684,37 @@
     <col min="2" max="2" width="17.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>84</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -1688,13 +1726,16 @@
         <v>4</v>
       </c>
       <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
         <v>8</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1708,15 +1749,18 @@
         <v>5</v>
       </c>
       <c r="E3" s="1">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1">
         <v>20</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
@@ -1728,15 +1772,18 @@
         <v>4</v>
       </c>
       <c r="E4" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
@@ -1748,36 +1795,42 @@
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -1788,13 +1841,16 @@
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1808,15 +1864,18 @@
         <v>1</v>
       </c>
       <c r="E8" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>5</v>
@@ -1828,14 +1887,17 @@
         <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F9" s="1">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F9"/>
+  <autoFilter ref="A1:G9"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>